<commit_message>
Update - Quality of Life Fixes
</commit_message>
<xml_diff>
--- a/UtilitiesReturns/Data/Config.xlsx
+++ b/UtilitiesReturns/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1006990\Downloads\UtilitiesReturns - Copy\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1006990\Downloads\UtilitiesReturns\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DFDEC2-1222-4EFC-A92F-031EA00612A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7233BDFF-6282-4101-9719-F16AA2AD2286}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -75,9 +75,6 @@
     <t>System exception.</t>
   </si>
   <si>
-    <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
     <t>OrchestratorQueueName</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -118,10 +115,13 @@
     <t>Completed Folder</t>
   </si>
   <si>
-    <t>In Progress Folder</t>
+    <t>Returns Folder</t>
   </si>
   <si>
-    <t>Returns Folder</t>
+    <t>In-Progress Folder</t>
+  </si>
+  <si>
+    <t>Workpackage Name</t>
   </si>
 </sst>
 </file>
@@ -494,7 +494,7 @@
   <dimension ref="A1:Y997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:D18"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -537,28 +537,28 @@
     </row>
     <row r="2" spans="1:25" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:25" ht="14.5">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:25" ht="14.25" customHeight="1">
       <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
         <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="14.25" customHeight="1"/>
@@ -1563,8 +1563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y987"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B14" sqref="A14:B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1666,25 +1666,25 @@
     <row r="11" spans="1:25" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:25" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
         <v>19</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:25" ht="14.25" customHeight="1">
       <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
         <v>24</v>
-      </c>
-      <c r="B14" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:25" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" t="b">
         <v>1</v>
@@ -1692,7 +1692,7 @@
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
@@ -2679,7 +2679,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:B8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2726,18 +2726,18 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -2750,34 +2750,34 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>